<commit_message>
improved writer code and added more migrations
</commit_message>
<xml_diff>
--- a/PoundPupLegacy.Convert/BasicSecondLevelSubdivisions.xlsx
+++ b/PoundPupLegacy.Convert/BasicSecondLevelSubdivisions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pd_af\source\repos\PoundPupLegacy\PoundPupLegacy.Convert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800E9380-C46C-4A25-8B67-CF2F442A8449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A46FF4-C05E-4CB5-9FF3-89409E8254A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8240" yWindow="5000" windowWidth="28810" windowHeight="15460" xr2:uid="{7820BEDA-216C-45D9-AF12-C83D70C48B86}"/>
+    <workbookView xWindow="13890" yWindow="4530" windowWidth="28830" windowHeight="15460" xr2:uid="{7820BEDA-216C-45D9-AF12-C83D70C48B86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4372" uniqueCount="3471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4416" uniqueCount="3505">
   <si>
     <t>Id</t>
   </si>
@@ -10447,6 +10447,108 @@
   </si>
   <si>
     <t>Tarfaya</t>
+  </si>
+  <si>
+    <t>Armagh City, Banbridge and Craigavon (Northern Irish district)</t>
+  </si>
+  <si>
+    <t>Armagh City, Banbridge and Craigavon</t>
+  </si>
+  <si>
+    <t>GB-WDU</t>
+  </si>
+  <si>
+    <t>GB-NIR</t>
+  </si>
+  <si>
+    <t>Ards and North Down (Northern Irish district)</t>
+  </si>
+  <si>
+    <t>Ards and North Down</t>
+  </si>
+  <si>
+    <t>GB-WFT</t>
+  </si>
+  <si>
+    <t>Antrim and Newtownabbey (Northern Irish district)</t>
+  </si>
+  <si>
+    <t>Antrim and Newtownabbey</t>
+  </si>
+  <si>
+    <t>GB-WGN</t>
+  </si>
+  <si>
+    <t>Belfast City (Northern Irish district)</t>
+  </si>
+  <si>
+    <t>Belfast City</t>
+  </si>
+  <si>
+    <t>GB-WKF</t>
+  </si>
+  <si>
+    <t>Causeway Coast and Glens (Northern Irish district)</t>
+  </si>
+  <si>
+    <t>Causeway Coast and Glens</t>
+  </si>
+  <si>
+    <t>GB-WLL</t>
+  </si>
+  <si>
+    <t>Derry and Strabane (Northern Irish district)</t>
+  </si>
+  <si>
+    <t>Derry and Strabane</t>
+  </si>
+  <si>
+    <t>GB-WLN</t>
+  </si>
+  <si>
+    <t>Fermanagh and Omagh (Northern Irish district)</t>
+  </si>
+  <si>
+    <t>Fermanagh and Omagh</t>
+  </si>
+  <si>
+    <t>GB-WRL</t>
+  </si>
+  <si>
+    <t>Lisburn and Castlereagh (Northern Irish district)</t>
+  </si>
+  <si>
+    <t>Lisburn and Castlereagh</t>
+  </si>
+  <si>
+    <t>GB-WRT</t>
+  </si>
+  <si>
+    <t>Mid and East Antrim (Northern Irish district)</t>
+  </si>
+  <si>
+    <t>Mid and East Antrim</t>
+  </si>
+  <si>
+    <t>GB-WRX</t>
+  </si>
+  <si>
+    <t>Mid-Ulster (Northern Irish district)</t>
+  </si>
+  <si>
+    <t>Mid-Ulster</t>
+  </si>
+  <si>
+    <t>GB-WSM</t>
+  </si>
+  <si>
+    <t>Newry, Mourne and Down (Northern Irish district)</t>
+  </si>
+  <si>
+    <t>Newry, Mourne and Down</t>
+  </si>
+  <si>
+    <t>GB-ZET</t>
   </si>
 </sst>
 </file>
@@ -10482,9 +10584,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10799,10 +10902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE658DB-E3AF-4E7C-89A8-5DC2E237B286}">
-  <dimension ref="A1:L1091"/>
+  <dimension ref="A1:L1102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A792" workbookViewId="0">
-      <selection activeCell="K809" sqref="K809"/>
+    <sheetView tabSelected="1" topLeftCell="A1066" workbookViewId="0">
+      <selection activeCell="H1102" sqref="H1102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -52272,6 +52375,424 @@
         <v>2999</v>
       </c>
     </row>
+    <row r="1092" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1092" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1092" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="C1092" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="D1092" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1092">
+        <v>17</v>
+      </c>
+      <c r="F1092">
+        <v>1</v>
+      </c>
+      <c r="G1092">
+        <v>1</v>
+      </c>
+      <c r="H1092">
+        <v>3992</v>
+      </c>
+      <c r="I1092" t="s">
+        <v>3471</v>
+      </c>
+      <c r="J1092" t="s">
+        <v>3472</v>
+      </c>
+      <c r="K1092" t="s">
+        <v>3473</v>
+      </c>
+      <c r="L1092" t="s">
+        <v>3474</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1093" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1093" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="C1093" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="D1093" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1093">
+        <v>17</v>
+      </c>
+      <c r="F1093">
+        <v>1</v>
+      </c>
+      <c r="G1093">
+        <v>1</v>
+      </c>
+      <c r="H1093">
+        <v>3992</v>
+      </c>
+      <c r="I1093" t="s">
+        <v>3475</v>
+      </c>
+      <c r="J1093" t="s">
+        <v>3476</v>
+      </c>
+      <c r="K1093" t="s">
+        <v>3477</v>
+      </c>
+      <c r="L1093" t="s">
+        <v>3474</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1094" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1094" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="C1094" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="D1094" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1094">
+        <v>17</v>
+      </c>
+      <c r="F1094">
+        <v>1</v>
+      </c>
+      <c r="G1094">
+        <v>1</v>
+      </c>
+      <c r="H1094">
+        <v>3992</v>
+      </c>
+      <c r="I1094" t="s">
+        <v>3478</v>
+      </c>
+      <c r="J1094" t="s">
+        <v>3479</v>
+      </c>
+      <c r="K1094" t="s">
+        <v>3480</v>
+      </c>
+      <c r="L1094" t="s">
+        <v>3474</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1095" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1095" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="C1095" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="D1095" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1095">
+        <v>17</v>
+      </c>
+      <c r="F1095">
+        <v>1</v>
+      </c>
+      <c r="G1095">
+        <v>1</v>
+      </c>
+      <c r="H1095">
+        <v>3992</v>
+      </c>
+      <c r="I1095" t="s">
+        <v>3481</v>
+      </c>
+      <c r="J1095" t="s">
+        <v>3482</v>
+      </c>
+      <c r="K1095" t="s">
+        <v>3483</v>
+      </c>
+      <c r="L1095" t="s">
+        <v>3474</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1096" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1096" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="C1096" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="D1096" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1096">
+        <v>17</v>
+      </c>
+      <c r="F1096">
+        <v>1</v>
+      </c>
+      <c r="G1096">
+        <v>1</v>
+      </c>
+      <c r="H1096">
+        <v>3992</v>
+      </c>
+      <c r="I1096" t="s">
+        <v>3484</v>
+      </c>
+      <c r="J1096" t="s">
+        <v>3485</v>
+      </c>
+      <c r="K1096" t="s">
+        <v>3486</v>
+      </c>
+      <c r="L1096" t="s">
+        <v>3474</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1097" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1097" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="C1097" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="D1097" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1097">
+        <v>17</v>
+      </c>
+      <c r="F1097">
+        <v>1</v>
+      </c>
+      <c r="G1097">
+        <v>1</v>
+      </c>
+      <c r="H1097">
+        <v>3992</v>
+      </c>
+      <c r="I1097" t="s">
+        <v>3487</v>
+      </c>
+      <c r="J1097" t="s">
+        <v>3488</v>
+      </c>
+      <c r="K1097" t="s">
+        <v>3489</v>
+      </c>
+      <c r="L1097" t="s">
+        <v>3474</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1098" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1098" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="C1098" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="D1098" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1098">
+        <v>17</v>
+      </c>
+      <c r="F1098">
+        <v>1</v>
+      </c>
+      <c r="G1098">
+        <v>1</v>
+      </c>
+      <c r="H1098">
+        <v>3992</v>
+      </c>
+      <c r="I1098" t="s">
+        <v>3490</v>
+      </c>
+      <c r="J1098" t="s">
+        <v>3491</v>
+      </c>
+      <c r="K1098" t="s">
+        <v>3492</v>
+      </c>
+      <c r="L1098" t="s">
+        <v>3474</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1099" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1099" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="C1099" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="D1099" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1099">
+        <v>17</v>
+      </c>
+      <c r="F1099">
+        <v>1</v>
+      </c>
+      <c r="G1099">
+        <v>1</v>
+      </c>
+      <c r="H1099">
+        <v>3992</v>
+      </c>
+      <c r="I1099" t="s">
+        <v>3493</v>
+      </c>
+      <c r="J1099" t="s">
+        <v>3494</v>
+      </c>
+      <c r="K1099" t="s">
+        <v>3495</v>
+      </c>
+      <c r="L1099" t="s">
+        <v>3474</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1100" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1100" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="C1100" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="D1100" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1100">
+        <v>17</v>
+      </c>
+      <c r="F1100">
+        <v>1</v>
+      </c>
+      <c r="G1100">
+        <v>1</v>
+      </c>
+      <c r="H1100">
+        <v>3992</v>
+      </c>
+      <c r="I1100" t="s">
+        <v>3496</v>
+      </c>
+      <c r="J1100" t="s">
+        <v>3497</v>
+      </c>
+      <c r="K1100" t="s">
+        <v>3498</v>
+      </c>
+      <c r="L1100" t="s">
+        <v>3474</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1101" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1101" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="C1101" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="D1101" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1101">
+        <v>17</v>
+      </c>
+      <c r="F1101">
+        <v>1</v>
+      </c>
+      <c r="G1101">
+        <v>1</v>
+      </c>
+      <c r="H1101">
+        <v>3992</v>
+      </c>
+      <c r="I1101" t="s">
+        <v>3499</v>
+      </c>
+      <c r="J1101" t="s">
+        <v>3500</v>
+      </c>
+      <c r="K1101" t="s">
+        <v>3501</v>
+      </c>
+      <c r="L1101" t="s">
+        <v>3474</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1102" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1102" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="C1102" s="1">
+        <v>44915.741666666669</v>
+      </c>
+      <c r="D1102" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1102">
+        <v>17</v>
+      </c>
+      <c r="F1102">
+        <v>1</v>
+      </c>
+      <c r="G1102">
+        <v>1</v>
+      </c>
+      <c r="H1102">
+        <v>3992</v>
+      </c>
+      <c r="I1102" t="s">
+        <v>3502</v>
+      </c>
+      <c r="J1102" t="s">
+        <v>3503</v>
+      </c>
+      <c r="K1102" t="s">
+        <v>3504</v>
+      </c>
+      <c r="L1102" t="s">
+        <v>3474</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>